<commit_message>
updated data in Book1.xlsx
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -17,11 +17,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$B$1:$B$997</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$B$1:$B$996</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="47" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="43">
   <si>
     <t>Video views</t>
   </si>
@@ -107,6 +107,60 @@
   </si>
   <si>
     <t>Sum of Video views</t>
+  </si>
+  <si>
+    <t>Edu</t>
+  </si>
+  <si>
+    <t>Ent</t>
+  </si>
+  <si>
+    <t>Ga</t>
+  </si>
+  <si>
+    <t>Co</t>
+  </si>
+  <si>
+    <t>Mo</t>
+  </si>
+  <si>
+    <t>Mu</t>
+  </si>
+  <si>
+    <t>Sh</t>
+  </si>
+  <si>
+    <t>Sp</t>
+  </si>
+  <si>
+    <t>Tr</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>AV</t>
   </si>
 </sst>
 </file>
@@ -5209,7 +5263,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="47" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0">
@@ -6305,7 +6359,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Video views" fld="0" baseField="1" baseItem="0"/>
+    <dataField name="Sum of Video views" fld="0" baseField="1" baseItem="16"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -6582,13 +6636,13 @@
   <dimension ref="A3:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
     <col min="5" max="6" width="9" customWidth="1"/>
@@ -6786,10 +6840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6800,7 +6854,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B1" s="7">
         <v>15003458141</v>
@@ -6808,7 +6862,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B2" s="7">
         <v>550112774315</v>
@@ -6816,7 +6870,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B3" s="7">
         <v>696614472899</v>
@@ -6824,7 +6878,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B4" s="7">
         <v>2527739309583</v>
@@ -6832,7 +6886,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B5" s="7">
         <v>544422509313</v>
@@ -6840,7 +6894,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B6" s="7">
         <v>717638899629</v>
@@ -6848,7 +6902,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B7" s="7">
         <v>201817545540</v>
@@ -6856,7 +6910,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B8" s="7">
         <v>15383255129</v>
@@ -6864,7 +6918,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B9" s="7">
         <v>3121477506633</v>
@@ -6880,7 +6934,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B11" s="7">
         <v>270391919347</v>
@@ -6888,7 +6942,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B12" s="7">
         <v>10862911785</v>
@@ -6896,7 +6950,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B13" s="7">
         <v>1265791201548</v>
@@ -6904,7 +6958,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B14" s="7">
         <v>44866745899</v>
@@ -6912,7 +6966,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B15" s="7">
         <v>66976747110</v>
@@ -6920,7 +6974,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B16" s="7">
         <v>446206826909</v>
@@ -6928,7 +6982,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B17" s="7">
         <v>147986290620</v>
@@ -6936,7 +6990,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B18" s="7">
         <v>33262717607</v>
@@ -6944,18 +6998,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B19" s="7">
         <v>3140883140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="7">
-        <v>10853130514846</v>
       </c>
     </row>
   </sheetData>
@@ -6965,10 +7011,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B997"/>
+  <dimension ref="A1:B996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A970" workbookViewId="0">
+      <selection activeCell="A996" sqref="A996"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7217,7 +7263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>59316472754</v>
       </c>
@@ -7281,7 +7327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>35302243691</v>
       </c>
@@ -7497,7 +7543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>36458726976</v>
       </c>
@@ -7657,7 +7703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>7339333120</v>
       </c>
@@ -7785,7 +7831,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>18961241905</v>
       </c>
@@ -7929,7 +7975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>11351015824</v>
       </c>
@@ -7945,7 +7991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>27274550757</v>
       </c>
@@ -7969,7 +8015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>13013567335</v>
       </c>
@@ -8065,7 +8111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>16613441479</v>
       </c>
@@ -8129,7 +8175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>5711208484</v>
       </c>
@@ -8185,7 +8231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>22919271731</v>
       </c>
@@ -8449,7 +8495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>13577142726</v>
       </c>
@@ -8497,7 +8543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>8603468420</v>
       </c>
@@ -8569,7 +8615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>22440611155</v>
       </c>
@@ -8665,7 +8711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>8595760553</v>
       </c>
@@ -8809,7 +8855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>2726917087</v>
       </c>
@@ -8977,7 +9023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <v>3647987299</v>
       </c>
@@ -9009,7 +9055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <v>6608773195</v>
       </c>
@@ -9097,7 +9143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="266" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
         <v>5652938599</v>
       </c>
@@ -9225,7 +9271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="282" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="2">
         <v>7920637200</v>
       </c>
@@ -9249,7 +9295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="2">
         <v>9465863821</v>
       </c>
@@ -9257,7 +9303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="286" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="2">
         <v>7926899136</v>
       </c>
@@ -9273,7 +9319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
         <v>2634</v>
       </c>
@@ -9345,7 +9391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
         <v>3378047383</v>
       </c>
@@ -9377,7 +9423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="2">
         <v>5380073627</v>
       </c>
@@ -9473,7 +9519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="2">
         <v>2431154438</v>
       </c>
@@ -9553,7 +9599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="323" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="2">
         <v>4454917643</v>
       </c>
@@ -9593,7 +9639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="2">
         <v>5614621131</v>
       </c>
@@ -9985,7 +10031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="377" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="2">
         <v>1796227417</v>
       </c>
@@ -10145,7 +10191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="397" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" s="2">
         <v>11317309935</v>
       </c>
@@ -10217,7 +10263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="406" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" s="2">
         <v>9715291883</v>
       </c>
@@ -10233,7 +10279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="408" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" s="2">
         <v>3234880084</v>
       </c>
@@ -10273,7 +10319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="413" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="2">
         <v>10955619815</v>
       </c>
@@ -10321,7 +10367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="419" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" s="2">
         <v>7906181776</v>
       </c>
@@ -10385,7 +10431,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="427" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" s="2">
         <v>2897907132</v>
       </c>
@@ -10393,7 +10439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="428" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" s="2">
         <v>4508184467</v>
       </c>
@@ -10433,7 +10479,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="433" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" s="2">
         <v>5194942269</v>
       </c>
@@ -10465,7 +10511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="437" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" s="2">
         <v>8281724393</v>
       </c>
@@ -10473,7 +10519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="438" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" s="2">
         <v>13824277846</v>
       </c>
@@ -10849,7 +10895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="485" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A485" s="2">
         <v>8716982055</v>
       </c>
@@ -10937,7 +10983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="496" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A496" s="2">
         <v>8588704539</v>
       </c>
@@ -11009,7 +11055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="505" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A505" s="2">
         <v>9059696049</v>
       </c>
@@ -11017,7 +11063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="506" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A506" s="2">
         <v>17247584185</v>
       </c>
@@ -11137,7 +11183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="521" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A521" s="2">
         <v>1026425106</v>
       </c>
@@ -11145,7 +11191,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="522" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" s="2">
         <v>902225615</v>
       </c>
@@ -11177,7 +11223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="526" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" s="2">
         <v>3606912471</v>
       </c>
@@ -11321,7 +11367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="544" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A544" s="2">
         <v>3523578665</v>
       </c>
@@ -11361,7 +11407,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="549" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A549" s="2">
         <v>3693798804</v>
       </c>
@@ -11825,7 +11871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="607" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A607" s="2">
         <v>5997599089</v>
       </c>
@@ -11913,7 +11959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="618" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" s="2">
         <v>13116313599</v>
       </c>
@@ -11921,7 +11967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="619" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A619" s="2">
         <v>9787697838</v>
       </c>
@@ -11985,7 +12031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="627" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A627" s="2">
         <v>7172386509</v>
       </c>
@@ -12057,7 +12103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="636" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="636" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A636" s="2">
         <v>12880388253</v>
       </c>
@@ -12121,7 +12167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="644" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A644" s="2">
         <v>3736069980</v>
       </c>
@@ -13105,7 +13151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="767" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="767" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A767" s="2">
         <v>9023952946</v>
       </c>
@@ -13153,7 +13199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="773" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="773" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A773" s="2">
         <v>4040297006</v>
       </c>
@@ -13273,7 +13319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="788" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="788" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A788" s="2">
         <v>5405563355</v>
       </c>
@@ -13417,7 +13463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="806" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="806" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A806" s="2">
         <v>2244318380</v>
       </c>
@@ -13497,7 +13543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="816" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="816" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A816" s="2">
         <v>1820559912</v>
       </c>
@@ -13865,7 +13911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="862" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="862" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A862" s="2">
         <v>2262690743</v>
       </c>
@@ -14057,7 +14103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="886" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A886" s="2">
         <v>1138262456</v>
       </c>
@@ -14129,7 +14175,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="895" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="895" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A895" s="2">
         <v>4214172991</v>
       </c>
@@ -14737,7 +14783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="971" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="971" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A971" s="2">
         <v>4340213066</v>
       </c>
@@ -14825,7 +14871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="982" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="982" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A982" s="2">
         <v>7683670251</v>
       </c>
@@ -14945,14 +14991,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="997" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A997" s="1">
-        <f>SUM(A2:A971)</f>
-        <v>10853130514846</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="B1:B997"/>
+  <autoFilter ref="B1:B996"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>